<commit_message>
PriceRange and other filters added.
</commit_message>
<xml_diff>
--- a/src/FormRegistration.xlsx
+++ b/src/FormRegistration.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Bookshelves</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -357,21 +360,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>15000</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>